<commit_message>
fixed reload cmd error & parsing of data
</commit_message>
<xml_diff>
--- a/documentation/Socketlist.xlsx
+++ b/documentation/Socketlist.xlsx
@@ -1290,16 +1290,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>126065</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>36418</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>72278</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>105065</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>140925</xdr:rowOff>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>15418</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>51278</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1308,7 +1308,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2692212" y="1495425"/>
+          <a:off x="4698065" y="2358278"/>
           <a:ext cx="360000" cy="360000"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -1405,15 +1405,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>14006</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>119343</xdr:rowOff>
+      <xdr:colOff>25212</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>108137</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>183506</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>98343</xdr:rowOff>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>4212</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>87137</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1422,7 +1422,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4675653" y="2595843"/>
+          <a:off x="4686859" y="2965637"/>
           <a:ext cx="360000" cy="360000"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -1519,14 +1519,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>12886</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:colOff>35298</xdr:colOff>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>6163</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>182386</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>14298</xdr:colOff>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>175663</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1536,7 +1536,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4674533" y="2292163"/>
+          <a:off x="4696945" y="2673163"/>
           <a:ext cx="360000" cy="360000"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -1577,14 +1577,14 @@
     <xdr:from>
       <xdr:col>22</xdr:col>
       <xdr:colOff>127747</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>179854</xdr:rowOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>101412</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
       <xdr:colOff>106747</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>158854</xdr:rowOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>80412</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1593,7 +1593,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4408394" y="2275354"/>
+          <a:off x="4408394" y="2958912"/>
           <a:ext cx="360000" cy="360000"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -1803,16 +1803,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>129988</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>47626</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>85165</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>36421</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>108988</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>26626</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>64165</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>15421</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1821,7 +1821,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2696135" y="1762126"/>
+          <a:off x="4365812" y="2322421"/>
           <a:ext cx="360000" cy="360000"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -1918,15 +1918,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>152398</xdr:colOff>
+      <xdr:colOff>107574</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>126069</xdr:rowOff>
+      <xdr:rowOff>182098</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>131398</xdr:colOff>
+      <xdr:colOff>86574</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>105069</xdr:rowOff>
+      <xdr:rowOff>161098</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1935,7 +1935,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4433045" y="2602569"/>
+          <a:off x="4388221" y="2658598"/>
           <a:ext cx="360000" cy="360000"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -2263,15 +2263,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>94129</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>560</xdr:rowOff>
+      <xdr:colOff>38099</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>561</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>73129</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>170060</xdr:rowOff>
+      <xdr:colOff>17099</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>170061</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2280,7 +2280,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4184276" y="2286560"/>
+          <a:off x="4128246" y="2477061"/>
           <a:ext cx="360000" cy="360000"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -3131,15 +3131,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>76201</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>128306</xdr:rowOff>
+      <xdr:colOff>31377</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>139512</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>55201</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>107306</xdr:rowOff>
+      <xdr:colOff>10377</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>118512</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3148,7 +3148,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4166348" y="2604806"/>
+          <a:off x="4121524" y="2806512"/>
           <a:ext cx="360000" cy="360000"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -3538,7 +3538,7 @@
   <dimension ref="A1:AO40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AD1" sqref="AD1"/>
+      <selection activeCell="AF1" sqref="AF1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3595,7 +3595,7 @@
         <v>28</v>
       </c>
       <c r="AH2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI2" t="s">
         <v>101</v>
@@ -3624,7 +3624,7 @@
         <v>95</v>
       </c>
       <c r="AH3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AI3" t="s">
         <v>101</v>
@@ -3656,7 +3656,7 @@
         <v>29</v>
       </c>
       <c r="AH4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AI4" t="s">
         <v>101</v>
@@ -3665,10 +3665,10 @@
         <v>3</v>
       </c>
       <c r="AK4">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="AL4">
-        <v>48</v>
+        <v>2</v>
       </c>
       <c r="AM4" t="s">
         <v>21</v>
@@ -3685,7 +3685,7 @@
         <v>89</v>
       </c>
       <c r="AH5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AI5" t="s">
         <v>101</v>
@@ -3717,7 +3717,7 @@
         <v>30</v>
       </c>
       <c r="AH6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AI6" t="s">
         <v>101</v>
@@ -3726,7 +3726,7 @@
         <v>5</v>
       </c>
       <c r="AK6">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="AL6">
         <v>2</v>
@@ -3746,7 +3746,7 @@
         <v>83</v>
       </c>
       <c r="AH7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AI7" t="s">
         <v>101</v>
@@ -3778,7 +3778,7 @@
         <v>31</v>
       </c>
       <c r="AH8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AI8" t="s">
         <v>101</v>
@@ -3787,7 +3787,7 @@
         <v>7</v>
       </c>
       <c r="AK8">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="AL8">
         <v>2</v>
@@ -3807,7 +3807,7 @@
         <v>77</v>
       </c>
       <c r="AH9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AI9" t="s">
         <v>101</v>
@@ -3839,7 +3839,7 @@
         <v>32</v>
       </c>
       <c r="AH10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="AI10" t="s">
         <v>29</v>
@@ -3868,7 +3868,7 @@
         <v>71</v>
       </c>
       <c r="AH11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AI11" t="s">
         <v>29</v>
@@ -3877,10 +3877,10 @@
         <v>2</v>
       </c>
       <c r="AK11">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="AL11">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="AM11" t="s">
         <v>47</v>
@@ -3900,7 +3900,7 @@
         <v>33</v>
       </c>
       <c r="AH12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="AI12" t="s">
         <v>29</v>
@@ -3929,7 +3929,7 @@
         <v>65</v>
       </c>
       <c r="AH13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AI13" t="s">
         <v>30</v>
@@ -3961,7 +3961,7 @@
         <v>34</v>
       </c>
       <c r="AH14">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="AI14" t="s">
         <v>30</v>
@@ -3970,10 +3970,10 @@
         <v>2</v>
       </c>
       <c r="AK14">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="AL14">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="AM14" t="s">
         <v>21</v>
@@ -3990,7 +3990,7 @@
         <v>60</v>
       </c>
       <c r="AH15">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="AI15" t="s">
         <v>30</v>
@@ -4022,7 +4022,7 @@
         <v>35</v>
       </c>
       <c r="AH16">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AI16" t="s">
         <v>44</v>
@@ -4034,7 +4034,7 @@
         <v>60</v>
       </c>
       <c r="AL16">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="AM16" t="s">
         <v>51</v>
@@ -4051,7 +4051,7 @@
         <v>55</v>
       </c>
       <c r="AH17">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AI17" t="s">
         <v>44</v>
@@ -4083,7 +4083,7 @@
         <v>36</v>
       </c>
       <c r="AH18">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AI18" t="s">
         <v>32</v>
@@ -4112,7 +4112,7 @@
         <v>50</v>
       </c>
       <c r="AH19">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="AI19" t="s">
         <v>32</v>
@@ -4144,7 +4144,7 @@
         <v>37</v>
       </c>
       <c r="AH20">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="AI20" t="s">
         <v>33</v>
@@ -4173,7 +4173,7 @@
         <v>45</v>
       </c>
       <c r="AH21">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="AI21" t="s">
         <v>34</v>
@@ -4182,10 +4182,10 @@
         <v>1</v>
       </c>
       <c r="AK21">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="AL21">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="AM21" t="s">
         <v>57</v>
@@ -4205,7 +4205,7 @@
         <v>38</v>
       </c>
       <c r="AH22">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="AI22" t="s">
         <v>34</v>
@@ -4234,7 +4234,7 @@
         <v>39</v>
       </c>
       <c r="AH23">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="AI23" t="s">
         <v>34</v>
@@ -4263,7 +4263,7 @@
         <v>36</v>
       </c>
       <c r="AH24">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="AI24" t="s">
         <v>34</v>
@@ -4292,7 +4292,7 @@
         <v>33</v>
       </c>
       <c r="AH25">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="AI25" t="s">
         <v>34</v>
@@ -4321,7 +4321,7 @@
         <v>30</v>
       </c>
       <c r="AH26">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AI26" t="s">
         <v>34</v>
@@ -4350,7 +4350,7 @@
         <v>27</v>
       </c>
       <c r="AH27">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="AI27" t="s">
         <v>34</v>
@@ -4379,7 +4379,7 @@
         <v>24</v>
       </c>
       <c r="AH28">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AI28" t="s">
         <v>35</v>
@@ -4408,7 +4408,7 @@
         <v>21</v>
       </c>
       <c r="AH29">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AI29" t="s">
         <v>35</v>
@@ -4437,7 +4437,7 @@
         <v>18</v>
       </c>
       <c r="AH30">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AI30" t="s">
         <v>35</v>
@@ -4466,7 +4466,7 @@
         <v>15</v>
       </c>
       <c r="AH31">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="AI31" t="s">
         <v>35</v>
@@ -4495,7 +4495,7 @@
         <v>12</v>
       </c>
       <c r="AH32">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AI32" t="s">
         <v>35</v>
@@ -4524,7 +4524,7 @@
         <v>10</v>
       </c>
       <c r="AH33">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AI33" t="s">
         <v>36</v>
@@ -4553,7 +4553,7 @@
         <v>8</v>
       </c>
       <c r="AH34">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AI34" t="s">
         <v>36</v>
@@ -4582,7 +4582,7 @@
         <v>5</v>
       </c>
       <c r="AH35">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AI35" t="s">
         <v>45</v>
@@ -4611,7 +4611,7 @@
         <v>2</v>
       </c>
       <c r="AH36">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AI36" t="s">
         <v>38</v>
@@ -4620,10 +4620,10 @@
         <v>1</v>
       </c>
       <c r="AK36">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AL36">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="AM36" t="s">
         <v>69</v>

</xml_diff>